<commit_message>
better handling Vector{T} type data
</commit_message>
<xml_diff>
--- a/test/data/examples.xlsx
+++ b/test/data/examples.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maste\.julia\dev\XLSXasJSON\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devsisters\.julia\dev\XLSXasJSON\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B12CD84-A72E-4C9B-8209-EFCA7126773B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4365" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4365" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="example1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="example5" sheetId="3" r:id="rId3"/>
     <sheet name="example6" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,11 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
-  <si>
-    <t>array1()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>array_int(Int)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -301,13 +296,21 @@
   </si>
   <si>
     <t>array_float(Float)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array_any()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array_string(String)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,50 +628,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="1" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
-        <v>76</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>900</v>
+      </c>
+      <c r="B4">
+        <v>900</v>
+      </c>
+      <c r="C4">
+        <v>900</v>
+      </c>
+      <c r="D4">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -679,77 +706,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D58AE00-CCEE-42A4-9CA2-E5EBEB570F4B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -759,93 +786,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970CF20F-2EFA-4C7B-9688-CC8412C2A4EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
-        <v>32</v>
-      </c>
       <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
       <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>54</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>55</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>56</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>57</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>58</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>59</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>61</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -853,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>0.55000000000000004</v>
@@ -865,67 +892,67 @@
         <v>1001</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>1002</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2">
         <v>1004</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2">
         <v>1003</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M2">
         <v>5001</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O2">
         <v>5002</v>
       </c>
       <c r="P2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q2">
         <v>5005</v>
       </c>
       <c r="R2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S2">
         <v>5007</v>
       </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U2">
         <v>5006</v>
       </c>
       <c r="V2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W2">
         <v>5003</v>
       </c>
       <c r="X2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y2">
         <v>5004</v>
       </c>
       <c r="Z2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -933,10 +960,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>0.55000000000000004</v>
@@ -945,37 +972,37 @@
         <v>1001</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3">
         <v>5001</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O3">
         <v>5002</v>
       </c>
       <c r="P3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q3">
         <v>5005</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S3">
         <v>5003</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U3">
         <v>5004</v>
       </c>
       <c r="V3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -983,10 +1010,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>0.55000000000000004</v>
@@ -995,37 +1022,37 @@
         <v>1001</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4">
         <v>1002</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4">
         <v>5001</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O4">
         <v>5002</v>
       </c>
       <c r="P4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q4">
         <v>5003</v>
       </c>
       <c r="R4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S4">
         <v>5004</v>
       </c>
       <c r="T4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1035,11 +1062,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5A62EA-ADF2-4118-A0C1-054C52D14A43}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1077,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1058,31 +1085,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -1090,7 +1117,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>2500</v>
@@ -1098,15 +1125,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>32</v>
@@ -1114,7 +1141,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9">
         <v>32</v>

</xml_diff>